<commit_message>
Adding All Team Template
</commit_message>
<xml_diff>
--- a/Management/Production_Progress_Templet.xlsx
+++ b/Management/Production_Progress_Templet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\GDC2017Project\Management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315"/>
+    <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Production Backlog Form" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="Sprint #3 Chart" sheetId="6" r:id="rId4"/>
     <sheet name="Sprint #4 Chart" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -497,7 +502,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1196,6 +1201,189 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1226,174 +1414,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1401,21 +1421,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1972,7 +1977,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2001,7 +2006,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2041,7 +2045,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D942-4F2E-B310-17B0B8FA8B33}"/>
             </c:ext>
@@ -2078,7 +2082,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D942-4F2E-B310-17B0B8FA8B33}"/>
             </c:ext>
@@ -2115,7 +2119,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D942-4F2E-B310-17B0B8FA8B33}"/>
             </c:ext>
@@ -2152,7 +2156,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-D942-4F2E-B310-17B0B8FA8B33}"/>
             </c:ext>
@@ -2212,7 +2216,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2228,7 +2231,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2284,7 +2287,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2327,7 +2330,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2370,7 +2373,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2413,7 +2416,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2468,7 +2471,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2484,7 +2486,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2540,7 +2542,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2583,7 +2585,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2626,7 +2628,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2669,7 +2671,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2724,7 +2726,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2740,7 +2741,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2796,7 +2797,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2839,7 +2840,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2882,7 +2883,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2925,7 +2926,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -2980,7 +2981,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2996,7 +2996,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3052,7 +3052,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -3095,7 +3095,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -3138,7 +3138,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -3181,7 +3181,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-ACDF-47F4-A593-ADC89855D2CF}"/>
             </c:ext>
@@ -3236,7 +3236,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3271,7 +3270,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3312,7 +3311,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56958FC8-1E61-451B-8A5B-94AA5987CCE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3355,7 +3354,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56958FC8-1E61-451B-8A5B-94AA5987CCE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3398,7 +3397,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56958FC8-1E61-451B-8A5B-94AA5987CCE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3441,7 +3440,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56958FC8-1E61-451B-8A5B-94AA5987CCE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3507,7 +3506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3540,9 +3539,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3575,6 +3591,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3753,8 +3786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3775,80 +3808,80 @@
   <sheetData>
     <row r="1" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
-      <c r="O2" s="132"/>
-      <c r="P2" s="133"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="120" t="s">
+      <c r="B3" s="111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="112"/>
+      <c r="D3" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="121"/>
-      <c r="J3" s="81" t="s">
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="118"/>
+      <c r="J3" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="83"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="101"/>
     </row>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="122" t="s">
+      <c r="C4" s="114"/>
+      <c r="D4" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="122"/>
-      <c r="H4" s="123"/>
-      <c r="J4" s="72" t="s">
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="120"/>
+      <c r="J4" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="74"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="104"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="119"/>
-      <c r="D5" s="124" t="s">
+      <c r="C5" s="116"/>
+      <c r="D5" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="125"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="122"/>
       <c r="J5" s="11" t="s">
         <v>66</v>
       </c>
@@ -3872,23 +3905,23 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="100"/>
-      <c r="J6" s="75" t="s">
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="66"/>
+      <c r="J6" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="77"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="106"/>
+      <c r="M6" s="106"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="107"/>
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
@@ -4101,14 +4134,14 @@
       <c r="H13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="78" t="s">
+      <c r="J13" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="80"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="110"/>
       <c r="P13" s="55"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
@@ -4210,15 +4243,15 @@
       <c r="P16" s="21"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="100"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="66"/>
       <c r="J17" s="12">
         <v>4</v>
       </c>
@@ -4234,15 +4267,15 @@
       <c r="P17" s="21"/>
     </row>
     <row r="18" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="106"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="81"/>
       <c r="J18" s="12">
         <v>5</v>
       </c>
@@ -4314,14 +4347,14 @@
         <f>SUM(E20:G20)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="130" t="s">
         <v>77</v>
       </c>
-      <c r="K20" s="70"/>
-      <c r="L20" s="70"/>
-      <c r="M20" s="70"/>
-      <c r="N20" s="70"/>
-      <c r="O20" s="71"/>
+      <c r="K20" s="131"/>
+      <c r="L20" s="131"/>
+      <c r="M20" s="131"/>
+      <c r="N20" s="131"/>
+      <c r="O20" s="132"/>
       <c r="P20" s="55"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
@@ -4395,13 +4428,13 @@
       <c r="P22" s="21"/>
     </row>
     <row r="23" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="109"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="84"/>
       <c r="J23" s="12">
         <v>3</v>
       </c>
@@ -4417,15 +4450,15 @@
       <c r="P23" s="21"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="99"/>
-      <c r="F24" s="99"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="100"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="66"/>
       <c r="J24" s="12">
         <v>4</v>
       </c>
@@ -4441,11 +4474,11 @@
       <c r="P24" s="21"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="126" t="s">
+      <c r="B25" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="127"/>
-      <c r="D25" s="127"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="10">
         <f>SUM(E28,E31,E34,E37)</f>
         <v>0</v>
@@ -4475,15 +4508,15 @@
       <c r="P25" s="21"/>
     </row>
     <row r="26" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="111" t="s">
+      <c r="B26" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="112"/>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="113"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="88"/>
       <c r="J26" s="13">
         <v>6</v>
       </c>
@@ -4502,33 +4535,33 @@
       <c r="B27" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="86"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="93" t="s">
+      <c r="C27" s="67"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="94"/>
-      <c r="G27" s="93" t="s">
+      <c r="F27" s="70"/>
+      <c r="G27" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="110"/>
+      <c r="H27" s="85"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="72" t="s">
+      <c r="J27" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
-      <c r="P27" s="74"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="103"/>
+      <c r="P27" s="104"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="86"/>
-      <c r="D28" s="87"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="9">
         <v>0</v>
       </c>
@@ -4566,40 +4599,40 @@
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="92"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="95"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="75" t="s">
+      <c r="J29" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="77"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="106"/>
+      <c r="M29" s="106"/>
+      <c r="N29" s="106"/>
+      <c r="O29" s="107"/>
       <c r="P29" s="21"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="84"/>
-      <c r="D30" s="85"/>
-      <c r="E30" s="93" t="s">
+      <c r="C30" s="89"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="F30" s="94"/>
-      <c r="G30" s="93" t="s">
+      <c r="F30" s="70"/>
+      <c r="G30" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="H30" s="110"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="1"/>
       <c r="J30" s="12">
         <v>1</v>
@@ -4619,8 +4652,8 @@
       <c r="B31" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="84"/>
-      <c r="D31" s="85"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
       <c r="E31" s="9">
         <v>0</v>
       </c>
@@ -4650,15 +4683,15 @@
       <c r="P31" s="21"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="92"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="95"/>
       <c r="I32" s="1"/>
       <c r="J32" s="12">
         <v>3</v>
@@ -4678,16 +4711,16 @@
       <c r="B33" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="86"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="93" t="s">
+      <c r="C33" s="67"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="94"/>
-      <c r="G33" s="93" t="s">
+      <c r="F33" s="70"/>
+      <c r="G33" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="H33" s="110"/>
+      <c r="H33" s="85"/>
       <c r="I33" s="1"/>
       <c r="J33" s="12">
         <v>4</v>
@@ -4707,8 +4740,8 @@
       <c r="B34" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="86"/>
-      <c r="D34" s="87"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="68"/>
       <c r="E34" s="9">
         <v>0</v>
       </c>
@@ -4738,15 +4771,15 @@
       <c r="P34" s="21"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B35" s="90" t="s">
+      <c r="B35" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="91"/>
-      <c r="H35" s="92"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="95"/>
       <c r="I35" s="1"/>
       <c r="J35" s="12">
         <v>6</v>
@@ -4766,33 +4799,33 @@
       <c r="B36" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="86"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="93" t="s">
+      <c r="C36" s="67"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="94"/>
-      <c r="G36" s="93" t="s">
+      <c r="F36" s="70"/>
+      <c r="G36" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="H36" s="110"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="78" t="s">
+      <c r="J36" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="79"/>
-      <c r="O36" s="80"/>
+      <c r="K36" s="109"/>
+      <c r="L36" s="109"/>
+      <c r="M36" s="109"/>
+      <c r="N36" s="109"/>
+      <c r="O36" s="110"/>
       <c r="P36" s="55"/>
     </row>
     <row r="37" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="88"/>
-      <c r="D37" s="89"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="92"/>
       <c r="E37" s="20">
         <v>0</v>
       </c>
@@ -4822,15 +4855,15 @@
       <c r="P37" s="21"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B38" s="98" t="s">
+      <c r="B38" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="100"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="66"/>
       <c r="I38" s="1"/>
       <c r="J38" s="12">
         <v>2</v>
@@ -4847,15 +4880,15 @@
       <c r="P38" s="21"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="95" t="s">
+      <c r="B39" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="96"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="96"/>
-      <c r="G39" s="96"/>
-      <c r="H39" s="97"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="1"/>
       <c r="J39" s="12">
         <v>3</v>
@@ -4872,15 +4905,15 @@
       <c r="P39" s="21"/>
     </row>
     <row r="40" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="101" t="s">
+      <c r="B40" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="102"/>
-      <c r="D40" s="102"/>
-      <c r="E40" s="102"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="102"/>
-      <c r="H40" s="103"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="78"/>
       <c r="I40" s="1"/>
       <c r="J40" s="12">
         <v>4</v>
@@ -4930,14 +4963,14 @@
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I43" s="1"/>
-      <c r="J43" s="69" t="s">
+      <c r="J43" s="130" t="s">
         <v>77</v>
       </c>
-      <c r="K43" s="70"/>
-      <c r="L43" s="70"/>
-      <c r="M43" s="70"/>
-      <c r="N43" s="70"/>
-      <c r="O43" s="71"/>
+      <c r="K43" s="131"/>
+      <c r="L43" s="131"/>
+      <c r="M43" s="131"/>
+      <c r="N43" s="131"/>
+      <c r="O43" s="132"/>
       <c r="P43" s="55"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
@@ -5038,15 +5071,15 @@
     </row>
     <row r="50" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I50" s="1"/>
-      <c r="J50" s="72" t="s">
+      <c r="J50" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="K50" s="73"/>
-      <c r="L50" s="73"/>
-      <c r="M50" s="73"/>
-      <c r="N50" s="73"/>
-      <c r="O50" s="73"/>
-      <c r="P50" s="74"/>
+      <c r="K50" s="103"/>
+      <c r="L50" s="103"/>
+      <c r="M50" s="103"/>
+      <c r="N50" s="103"/>
+      <c r="O50" s="103"/>
+      <c r="P50" s="104"/>
     </row>
     <row r="51" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I51" s="1"/>
@@ -5074,14 +5107,14 @@
     </row>
     <row r="52" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I52" s="1"/>
-      <c r="J52" s="75" t="s">
+      <c r="J52" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="K52" s="76"/>
-      <c r="L52" s="76"/>
-      <c r="M52" s="76"/>
-      <c r="N52" s="76"/>
-      <c r="O52" s="77"/>
+      <c r="K52" s="106"/>
+      <c r="L52" s="106"/>
+      <c r="M52" s="106"/>
+      <c r="N52" s="106"/>
+      <c r="O52" s="107"/>
       <c r="P52" s="21"/>
     </row>
     <row r="53" spans="9:16" x14ac:dyDescent="0.2">
@@ -5182,14 +5215,14 @@
     </row>
     <row r="59" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I59" s="1"/>
-      <c r="J59" s="78" t="s">
+      <c r="J59" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="K59" s="79"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="79"/>
-      <c r="N59" s="79"/>
-      <c r="O59" s="80"/>
+      <c r="K59" s="109"/>
+      <c r="L59" s="109"/>
+      <c r="M59" s="109"/>
+      <c r="N59" s="109"/>
+      <c r="O59" s="110"/>
       <c r="P59" s="55"/>
     </row>
     <row r="60" spans="9:16" x14ac:dyDescent="0.2">
@@ -5290,14 +5323,14 @@
     </row>
     <row r="66" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I66" s="1"/>
-      <c r="J66" s="69" t="s">
+      <c r="J66" s="130" t="s">
         <v>77</v>
       </c>
-      <c r="K66" s="70"/>
-      <c r="L66" s="70"/>
-      <c r="M66" s="70"/>
-      <c r="N66" s="70"/>
-      <c r="O66" s="71"/>
+      <c r="K66" s="131"/>
+      <c r="L66" s="131"/>
+      <c r="M66" s="131"/>
+      <c r="N66" s="131"/>
+      <c r="O66" s="132"/>
       <c r="P66" s="55"/>
     </row>
     <row r="67" spans="9:16" x14ac:dyDescent="0.2">
@@ -5398,15 +5431,15 @@
     </row>
     <row r="73" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I73" s="1"/>
-      <c r="J73" s="72" t="s">
+      <c r="J73" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="K73" s="73"/>
-      <c r="L73" s="73"/>
-      <c r="M73" s="73"/>
-      <c r="N73" s="73"/>
-      <c r="O73" s="73"/>
-      <c r="P73" s="74"/>
+      <c r="K73" s="103"/>
+      <c r="L73" s="103"/>
+      <c r="M73" s="103"/>
+      <c r="N73" s="103"/>
+      <c r="O73" s="103"/>
+      <c r="P73" s="104"/>
     </row>
     <row r="74" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I74" s="1"/>
@@ -5434,14 +5467,14 @@
     </row>
     <row r="75" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I75" s="1"/>
-      <c r="J75" s="75" t="s">
+      <c r="J75" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="K75" s="76"/>
-      <c r="L75" s="76"/>
-      <c r="M75" s="76"/>
-      <c r="N75" s="76"/>
-      <c r="O75" s="77"/>
+      <c r="K75" s="106"/>
+      <c r="L75" s="106"/>
+      <c r="M75" s="106"/>
+      <c r="N75" s="106"/>
+      <c r="O75" s="107"/>
       <c r="P75" s="21"/>
     </row>
     <row r="76" spans="9:16" x14ac:dyDescent="0.2">
@@ -5542,14 +5575,14 @@
     </row>
     <row r="82" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I82" s="1"/>
-      <c r="J82" s="78" t="s">
+      <c r="J82" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="K82" s="79"/>
-      <c r="L82" s="79"/>
-      <c r="M82" s="79"/>
-      <c r="N82" s="79"/>
-      <c r="O82" s="80"/>
+      <c r="K82" s="109"/>
+      <c r="L82" s="109"/>
+      <c r="M82" s="109"/>
+      <c r="N82" s="109"/>
+      <c r="O82" s="110"/>
       <c r="P82" s="55"/>
     </row>
     <row r="83" spans="9:16" x14ac:dyDescent="0.2">
@@ -5650,14 +5683,14 @@
     </row>
     <row r="89" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I89" s="1"/>
-      <c r="J89" s="69" t="s">
+      <c r="J89" s="130" t="s">
         <v>77</v>
       </c>
-      <c r="K89" s="70"/>
-      <c r="L89" s="70"/>
-      <c r="M89" s="70"/>
-      <c r="N89" s="70"/>
-      <c r="O89" s="71"/>
+      <c r="K89" s="131"/>
+      <c r="L89" s="131"/>
+      <c r="M89" s="131"/>
+      <c r="N89" s="131"/>
+      <c r="O89" s="132"/>
       <c r="P89" s="55"/>
     </row>
     <row r="90" spans="9:16" x14ac:dyDescent="0.2">
@@ -5758,47 +5791,69 @@
     </row>
     <row r="96" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I96" s="1"/>
-      <c r="J96" s="64" t="s">
+      <c r="J96" s="125" t="s">
         <v>71</v>
       </c>
-      <c r="K96" s="65"/>
-      <c r="L96" s="65"/>
-      <c r="M96" s="65"/>
-      <c r="N96" s="65"/>
-      <c r="O96" s="65"/>
-      <c r="P96" s="66"/>
+      <c r="K96" s="126"/>
+      <c r="L96" s="126"/>
+      <c r="M96" s="126"/>
+      <c r="N96" s="126"/>
+      <c r="O96" s="126"/>
+      <c r="P96" s="127"/>
     </row>
     <row r="97" spans="9:16" x14ac:dyDescent="0.2">
       <c r="I97" s="1"/>
       <c r="J97" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="K97" s="62" t="s">
+      <c r="K97" s="123" t="s">
         <v>75</v>
       </c>
-      <c r="L97" s="62"/>
-      <c r="M97" s="62"/>
-      <c r="N97" s="62"/>
-      <c r="O97" s="62"/>
-      <c r="P97" s="63"/>
+      <c r="L97" s="123"/>
+      <c r="M97" s="123"/>
+      <c r="N97" s="123"/>
+      <c r="O97" s="123"/>
+      <c r="P97" s="124"/>
     </row>
     <row r="98" spans="9:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J98" s="13"/>
-      <c r="K98" s="67"/>
-      <c r="L98" s="67"/>
-      <c r="M98" s="67"/>
-      <c r="N98" s="67"/>
-      <c r="O98" s="67"/>
-      <c r="P98" s="68"/>
+      <c r="K98" s="128"/>
+      <c r="L98" s="128"/>
+      <c r="M98" s="128"/>
+      <c r="N98" s="128"/>
+      <c r="O98" s="128"/>
+      <c r="P98" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="K97:P97"/>
+    <mergeCell ref="J96:P96"/>
+    <mergeCell ref="K98:P98"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="J36:O36"/>
+    <mergeCell ref="J43:O43"/>
+    <mergeCell ref="J82:O82"/>
+    <mergeCell ref="J89:O89"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="J66:O66"/>
+    <mergeCell ref="J73:P73"/>
+    <mergeCell ref="J75:O75"/>
+    <mergeCell ref="J52:O52"/>
+    <mergeCell ref="J50:P50"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D5:H5"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B23:H23"/>
@@ -5815,40 +5870,18 @@
     <mergeCell ref="B29:H29"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B38:H38"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="K97:P97"/>
-    <mergeCell ref="J96:P96"/>
-    <mergeCell ref="K98:P98"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="J36:O36"/>
-    <mergeCell ref="J43:O43"/>
-    <mergeCell ref="J82:O82"/>
-    <mergeCell ref="J89:O89"/>
-    <mergeCell ref="J59:O59"/>
-    <mergeCell ref="J66:O66"/>
-    <mergeCell ref="J73:P73"/>
-    <mergeCell ref="J75:O75"/>
-    <mergeCell ref="J52:O52"/>
-    <mergeCell ref="J50:P50"/>
   </mergeCells>
   <conditionalFormatting sqref="H20:H22">
     <cfRule type="cellIs" dxfId="56" priority="2" operator="between">
@@ -5879,8 +5912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5901,52 +5934,52 @@
   <sheetData>
     <row r="1" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="133" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="130"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="135"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="127"/>
+      <c r="D3" s="125" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="I3" s="64" t="s">
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
+      <c r="I3" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="66"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="127"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -6095,10 +6128,10 @@
       <c r="T7" s="36"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="125" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="127"/>
       <c r="D8" s="40" t="s">
         <v>16</v>
       </c>
@@ -6225,10 +6258,10 @@
       <c r="T11" s="36"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="127"/>
       <c r="D12" s="40" t="s">
         <v>24</v>
       </c>
@@ -6385,10 +6418,10 @@
       <c r="T17" s="36"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="127"/>
       <c r="I18" s="40" t="s">
         <v>144</v>
       </c>
@@ -6503,15 +6536,15 @@
       <c r="T22" s="39"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="135"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="63"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
@@ -6532,7 +6565,7 @@
       <c r="G24" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="135"/>
+      <c r="H24" s="63"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="40">
@@ -6555,7 +6588,7 @@
         <f>(COUNTA(I5:I22)-COUNTBLANK(J5:J22)) - F25</f>
         <v>0</v>
       </c>
-      <c r="H25" s="134"/>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="40">
@@ -6578,7 +6611,7 @@
         <f>G25-F26</f>
         <v>0</v>
       </c>
-      <c r="H26" s="134"/>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="40">
@@ -6601,7 +6634,7 @@
         <f t="shared" ref="G27:G31" si="3">G26-F27</f>
         <v>0</v>
       </c>
-      <c r="H27" s="134"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="40">
@@ -6624,7 +6657,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H28" s="134"/>
+      <c r="H28" s="62"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="40">
@@ -6647,7 +6680,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H29" s="134"/>
+      <c r="H29" s="62"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="40">
@@ -6670,7 +6703,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H30" s="134"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="42">
@@ -6693,7 +6726,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="134"/>
+      <c r="H31" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6796,52 +6829,52 @@
   <sheetData>
     <row r="1" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="133" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="130"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="135"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="127"/>
+      <c r="D3" s="125" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="I3" s="64" t="s">
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
+      <c r="I3" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="66"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="127"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -6990,10 +7023,10 @@
       <c r="T7" s="36"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="125" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="127"/>
       <c r="D8" s="40" t="s">
         <v>16</v>
       </c>
@@ -7120,10 +7153,10 @@
       <c r="T11" s="36"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="127"/>
       <c r="D12" s="40" t="s">
         <v>24</v>
       </c>
@@ -7280,10 +7313,10 @@
       <c r="T17" s="36"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="127"/>
       <c r="I18" s="40" t="s">
         <v>144</v>
       </c>
@@ -7398,15 +7431,15 @@
       <c r="T22" s="39"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="135"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="63"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
@@ -7427,7 +7460,7 @@
       <c r="G24" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="135"/>
+      <c r="H24" s="63"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="40">
@@ -7450,7 +7483,7 @@
         <f>(COUNTA(I5:I22)-COUNTBLANK(J5:J22)) - F25</f>
         <v>0</v>
       </c>
-      <c r="H25" s="134"/>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="40">
@@ -7473,7 +7506,7 @@
         <f>G25-F26</f>
         <v>0</v>
       </c>
-      <c r="H26" s="134"/>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="40">
@@ -7496,7 +7529,7 @@
         <f t="shared" ref="G27:G31" si="3">G26-F27</f>
         <v>0</v>
       </c>
-      <c r="H27" s="134"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="40">
@@ -7519,7 +7552,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H28" s="134"/>
+      <c r="H28" s="62"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="40">
@@ -7542,7 +7575,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H29" s="134"/>
+      <c r="H29" s="62"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="40">
@@ -7565,7 +7598,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H30" s="134"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="42">
@@ -7588,7 +7621,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="134"/>
+      <c r="H31" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -7688,52 +7721,52 @@
   <sheetData>
     <row r="1" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="133" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="130"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="135"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="127"/>
+      <c r="D3" s="125" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="I3" s="64" t="s">
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
+      <c r="I3" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="66"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="127"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -7882,10 +7915,10 @@
       <c r="T7" s="36"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="125" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="127"/>
       <c r="D8" s="40" t="s">
         <v>16</v>
       </c>
@@ -8012,10 +8045,10 @@
       <c r="T11" s="36"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="127"/>
       <c r="D12" s="40" t="s">
         <v>24</v>
       </c>
@@ -8172,10 +8205,10 @@
       <c r="T17" s="36"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="127"/>
       <c r="I18" s="40" t="s">
         <v>144</v>
       </c>
@@ -8290,15 +8323,15 @@
       <c r="T22" s="39"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="135"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="63"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
@@ -8319,7 +8352,7 @@
       <c r="G24" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="135"/>
+      <c r="H24" s="63"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="40">
@@ -8342,7 +8375,7 @@
         <f>(COUNTA(I5:I22)-COUNTBLANK(J5:J22)) - F25</f>
         <v>0</v>
       </c>
-      <c r="H25" s="134"/>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="40">
@@ -8365,7 +8398,7 @@
         <f>G25-F26</f>
         <v>0</v>
       </c>
-      <c r="H26" s="134"/>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="40">
@@ -8388,7 +8421,7 @@
         <f t="shared" ref="G27:G31" si="3">G26-F27</f>
         <v>0</v>
       </c>
-      <c r="H27" s="134"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="40">
@@ -8411,7 +8444,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H28" s="134"/>
+      <c r="H28" s="62"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="40">
@@ -8434,7 +8467,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H29" s="134"/>
+      <c r="H29" s="62"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="40">
@@ -8457,7 +8490,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H30" s="134"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="42">
@@ -8480,7 +8513,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="134"/>
+      <c r="H31" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -8580,52 +8613,52 @@
   <sheetData>
     <row r="1" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="133" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="130"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
+      <c r="R2" s="134"/>
+      <c r="S2" s="134"/>
+      <c r="T2" s="135"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="64" t="s">
+      <c r="C3" s="127"/>
+      <c r="D3" s="125" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="I3" s="64" t="s">
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
+      <c r="I3" s="125" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="66"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="127"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="35" t="s">
@@ -8774,10 +8807,10 @@
       <c r="T7" s="36"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="125" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="127"/>
       <c r="D8" s="40" t="s">
         <v>16</v>
       </c>
@@ -8904,10 +8937,10 @@
       <c r="T11" s="36"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="127"/>
       <c r="D12" s="40" t="s">
         <v>24</v>
       </c>
@@ -9064,10 +9097,10 @@
       <c r="T17" s="36"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="127"/>
       <c r="I18" s="40" t="s">
         <v>144</v>
       </c>
@@ -9182,15 +9215,15 @@
       <c r="T22" s="39"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="125" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="135"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="63"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
@@ -9211,7 +9244,7 @@
       <c r="G24" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="135"/>
+      <c r="H24" s="63"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="40">
@@ -9234,7 +9267,7 @@
         <f>(COUNTA(I5:I22)-COUNTBLANK(J5:J22)) - F25</f>
         <v>0</v>
       </c>
-      <c r="H25" s="134"/>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="40">
@@ -9257,7 +9290,7 @@
         <f>G25-F26</f>
         <v>0</v>
       </c>
-      <c r="H26" s="134"/>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="40">
@@ -9280,7 +9313,7 @@
         <f t="shared" ref="G27:G31" si="3">G26-F27</f>
         <v>0</v>
       </c>
-      <c r="H27" s="134"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="40">
@@ -9303,7 +9336,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H28" s="134"/>
+      <c r="H28" s="62"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="40">
@@ -9326,7 +9359,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H29" s="134"/>
+      <c r="H29" s="62"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="40">
@@ -9349,7 +9382,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H30" s="134"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="2:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="42">
@@ -9372,7 +9405,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="134"/>
+      <c r="H31" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>